<commit_message>
AG: ejemplo de diccionario
</commit_message>
<xml_diff>
--- a/04_Entregable 2/previo/metadatos y diccionario_AG.xlsx
+++ b/04_Entregable 2/previo/metadatos y diccionario_AG.xlsx
@@ -9,12 +9,14 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28770" windowHeight="11385" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28770" windowHeight="11385" firstSheet="2" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Metadatos generales" sheetId="1" r:id="rId1"/>
     <sheet name="Hoja2" sheetId="2" r:id="rId2"/>
-    <sheet name="02_1" sheetId="3" r:id="rId3"/>
+    <sheet name="02_1_general" sheetId="4" r:id="rId3"/>
+    <sheet name="02_1_diccionario" sheetId="3" r:id="rId4"/>
+    <sheet name="02_1_dominios" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -26,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="119">
   <si>
     <t>Elemento</t>
   </si>
@@ -164,9 +166,6 @@
   </si>
   <si>
     <t>VAR_001</t>
-  </si>
-  <si>
-    <t>Nombre científico de la especia traficada</t>
   </si>
   <si>
     <t>Texto (máximo 100 caracteres)</t>
@@ -224,9 +223,6 @@
     <t>Código alfanumérico de entre 14 y 15 caractéres</t>
   </si>
   <si>
-    <t>Judicatura</t>
-  </si>
-  <si>
     <t>variable de clasificación</t>
   </si>
   <si>
@@ -245,9 +241,6 @@
     <t>date</t>
   </si>
   <si>
-    <t>dd/mm/aaaa</t>
-  </si>
-  <si>
     <t>variable temporal</t>
   </si>
   <si>
@@ -260,9 +253,6 @@
     <t>Provincia donde se ingresa el juicio</t>
   </si>
   <si>
-    <t>Texto alfabético asociado con una de las 24 provincias del Ecuador</t>
-  </si>
-  <si>
     <t>variable de ubicación</t>
   </si>
   <si>
@@ -278,9 +268,6 @@
     <t>Cantón donde se ingresa el juicio</t>
   </si>
   <si>
-    <t>Texto alfabético asociado con uno de los 223 cantones de Ecuador</t>
-  </si>
-  <si>
     <t>LA LIBERTAD</t>
   </si>
   <si>
@@ -293,9 +280,6 @@
     <t>Lugar en el que se ingresa el juicio</t>
   </si>
   <si>
-    <t>Texto alfabético referente al lugar donde se ingresa el juicio</t>
-  </si>
-  <si>
     <t>UNIDAD JUDICIAL</t>
   </si>
   <si>
@@ -305,9 +289,6 @@
     <t>Tipo de delito cometido</t>
   </si>
   <si>
-    <t>Texto alfabético que describe el delito por el que sucede el juicio</t>
-  </si>
-  <si>
     <t>247 DELITOS CONTRA LA FLORA Y FAUNA SILVESTRES</t>
   </si>
   <si>
@@ -323,10 +304,88 @@
     <t>Estado del juicio ingresado</t>
   </si>
   <si>
-    <t>Texto alfabético que describe el estado del juicio</t>
-  </si>
-  <si>
     <t>RESUELTA</t>
+  </si>
+  <si>
+    <t>Debe ser un cantón de la provincia asignada</t>
+  </si>
+  <si>
+    <t>Nombre científico de la especie traficada</t>
+  </si>
+  <si>
+    <t>División político administrativa</t>
+  </si>
+  <si>
+    <t>Nombre del archivo</t>
+  </si>
+  <si>
+    <t>Formato</t>
+  </si>
+  <si>
+    <t>Hoja</t>
+  </si>
+  <si>
+    <t>Rango</t>
+  </si>
+  <si>
+    <t>Membrete</t>
+  </si>
+  <si>
+    <t>Procendencia</t>
+  </si>
+  <si>
+    <t>Frecuencia de actualización</t>
+  </si>
+  <si>
+    <t>CJ 0936 Causas Art 247 corte agosto 2024(1)</t>
+  </si>
+  <si>
+    <t>xlsx</t>
+  </si>
+  <si>
+    <t>Causas Ingresadas</t>
+  </si>
+  <si>
+    <t>CONSEJO DE LA JUDICATURA</t>
+  </si>
+  <si>
+    <t>DIRECCIÓN NACIONAL DE ESTUDIOS JURIMÉTRICOS Y ESTADÍSTICA JUDICIAL</t>
+  </si>
+  <si>
+    <t>CAUSAS INGRESADAS</t>
+  </si>
+  <si>
+    <t>2019 A AGOSTO 2024</t>
+  </si>
+  <si>
+    <t>B6:H250</t>
+  </si>
+  <si>
+    <t>Sistema Automático de Trámite Judicial Ecuatoriano (SATJE)</t>
+  </si>
+  <si>
+    <t>Fecha</t>
+  </si>
+  <si>
+    <t>Fechas en formato dd/mm/aaaa comprendidas entre 01/01/2019 hasta 31/08/2024</t>
+  </si>
+  <si>
+    <t>VALORES DIFERENTES A LOS PRESENTES EN LA BASE</t>
+  </si>
+  <si>
+    <t>Valores</t>
+  </si>
+  <si>
+    <t>DPA por año</t>
+  </si>
+  <si>
+    <t>CORTE NACIONAL</t>
+  </si>
+  <si>
+    <t>SALA DE CORTE PROVINCIAL</t>
+  </si>
+  <si>
+    <t>TRIBUNAL PENAL</t>
   </si>
 </sst>
 </file>
@@ -350,7 +409,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -372,6 +431,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -403,7 +468,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -439,6 +504,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -722,7 +792,7 @@
   <dimension ref="A2:B7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -790,7 +860,7 @@
   <dimension ref="A2:C19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:A19"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -841,7 +911,7 @@
         <v>30</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>46</v>
+        <v>93</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="30" x14ac:dyDescent="0.25">
@@ -852,7 +922,7 @@
         <v>31</v>
       </c>
       <c r="C6" s="10" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -863,7 +933,7 @@
         <v>32</v>
       </c>
       <c r="C7" s="10" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -874,29 +944,29 @@
         <v>33</v>
       </c>
       <c r="C8" s="10" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="B9" s="17" t="s">
+        <v>34</v>
+      </c>
+      <c r="C9" s="17" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="B9" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="C9" s="7" t="s">
+    <row r="10" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A10" s="17" t="s">
+        <v>19</v>
+      </c>
+      <c r="B10" s="17" t="s">
+        <v>35</v>
+      </c>
+      <c r="C10" s="17" t="s">
         <v>50</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A10" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="B10" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="C10" s="7" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
@@ -907,7 +977,7 @@
         <v>36</v>
       </c>
       <c r="C11" s="10" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
@@ -919,22 +989,22 @@
       <c r="A13" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="B13" s="10" t="s">
+      <c r="B13" s="7" t="s">
         <v>37</v>
       </c>
       <c r="C13" s="10" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A14" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="B14" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="C14" s="11" t="s">
         <v>53</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A14" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="B14" s="10" t="s">
-        <v>38</v>
-      </c>
-      <c r="C14" s="10" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="30" x14ac:dyDescent="0.25">
@@ -945,7 +1015,7 @@
         <v>39</v>
       </c>
       <c r="C15" s="10" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="60" x14ac:dyDescent="0.25">
@@ -956,29 +1026,29 @@
         <v>40</v>
       </c>
       <c r="C16" s="11" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A17" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="B17" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="C17" s="7" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A17" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="B17" s="10" t="s">
-        <v>41</v>
-      </c>
-      <c r="C17" s="10" t="s">
+    <row r="18" spans="1:3" ht="75" x14ac:dyDescent="0.25">
+      <c r="A18" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="B18" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="C18" s="7" t="s">
         <v>57</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" ht="75" x14ac:dyDescent="0.25">
-      <c r="A18" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="B18" s="10" t="s">
-        <v>42</v>
-      </c>
-      <c r="C18" s="10" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="135" x14ac:dyDescent="0.25">
@@ -989,7 +1059,7 @@
         <v>43</v>
       </c>
       <c r="C19" s="10" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
   </sheetData>
@@ -1000,10 +1070,98 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O8"/>
+  <dimension ref="A1:E8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="25.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>95</v>
+      </c>
+      <c r="B1" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>96</v>
+      </c>
+      <c r="B2" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>97</v>
+      </c>
+      <c r="B3" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>99</v>
+      </c>
+      <c r="B4" t="s">
+        <v>105</v>
+      </c>
+      <c r="C4" t="s">
+        <v>106</v>
+      </c>
+      <c r="D4" t="s">
+        <v>107</v>
+      </c>
+      <c r="E4" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>98</v>
+      </c>
+      <c r="B5" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>100</v>
+      </c>
+      <c r="B6" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>111</v>
+      </c>
+      <c r="B7" s="14">
+        <v>45535</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>101</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="A2" sqref="A2:A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1011,21 +1169,17 @@
     <col min="1" max="1" width="21.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="17.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="28.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="43.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="22.28515625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="25.7109375" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.7109375" style="15" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="22.28515625" style="15" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="16.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="13" t="s">
         <v>12</v>
       </c>
@@ -1035,265 +1189,305 @@
       <c r="C1" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="D1" s="13" t="s">
+      <c r="D1" s="16" t="s">
         <v>15</v>
       </c>
       <c r="E1" s="13" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="F1" s="13" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="G1" s="13" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="H1" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="I1" s="13" t="s">
         <v>20</v>
       </c>
+      <c r="I1" s="16" t="s">
+        <v>21</v>
+      </c>
       <c r="J1" s="13" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="K1" s="13" t="s">
-        <v>22</v>
-      </c>
-      <c r="L1" s="13" t="s">
-        <v>23</v>
-      </c>
-      <c r="M1" s="13" t="s">
-        <v>25</v>
-      </c>
-      <c r="N1" s="13" t="s">
-        <v>26</v>
-      </c>
-      <c r="O1" s="13" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>60</v>
+      </c>
+      <c r="B2" t="s">
+        <v>59</v>
+      </c>
+      <c r="C2" t="s">
         <v>61</v>
       </c>
+      <c r="D2" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="E2" t="s">
+        <v>48</v>
+      </c>
+      <c r="F2" t="s">
+        <v>48</v>
+      </c>
+      <c r="H2" s="15" t="s">
+        <v>63</v>
+      </c>
+      <c r="I2" s="15" t="s">
+        <v>52</v>
+      </c>
+      <c r="J2" s="12" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>66</v>
+      </c>
+      <c r="B3" t="s">
+        <v>67</v>
+      </c>
+      <c r="C3" t="s">
+        <v>68</v>
+      </c>
+      <c r="D3" s="15" t="s">
+        <v>69</v>
+      </c>
+      <c r="E3" t="s">
+        <v>48</v>
+      </c>
+      <c r="F3" t="s">
+        <v>48</v>
+      </c>
+      <c r="H3" t="s">
+        <v>112</v>
+      </c>
+      <c r="I3" s="15" t="s">
+        <v>70</v>
+      </c>
+      <c r="J3" s="14">
+        <v>43742</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>71</v>
+      </c>
+      <c r="B4" t="s">
+        <v>72</v>
+      </c>
+      <c r="C4" t="s">
+        <v>73</v>
+      </c>
+      <c r="D4" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="E4" t="s">
+        <v>48</v>
+      </c>
+      <c r="F4" t="s">
+        <v>94</v>
+      </c>
+      <c r="H4" t="s">
+        <v>51</v>
+      </c>
+      <c r="I4" s="15" t="s">
+        <v>74</v>
+      </c>
+      <c r="J4" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>76</v>
+      </c>
+      <c r="B5" t="s">
+        <v>77</v>
+      </c>
+      <c r="C5" t="s">
+        <v>78</v>
+      </c>
+      <c r="D5" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="E5" t="s">
+        <v>48</v>
+      </c>
+      <c r="F5" t="s">
+        <v>94</v>
+      </c>
+      <c r="G5" t="s">
+        <v>72</v>
+      </c>
+      <c r="H5" t="s">
+        <v>92</v>
+      </c>
+      <c r="I5" s="15" t="s">
+        <v>74</v>
+      </c>
+      <c r="J5" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>80</v>
+      </c>
+      <c r="B6" t="s">
+        <v>81</v>
+      </c>
+      <c r="C6" t="s">
+        <v>82</v>
+      </c>
+      <c r="D6" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="E6" t="s">
+        <v>48</v>
+      </c>
+      <c r="F6" s="15"/>
+      <c r="I6" s="15" t="s">
+        <v>74</v>
+      </c>
+      <c r="J6" t="s">
+        <v>83</v>
+      </c>
+      <c r="K6" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>87</v>
+      </c>
+      <c r="B7" t="s">
+        <v>84</v>
+      </c>
+      <c r="C7" t="s">
+        <v>85</v>
+      </c>
+      <c r="D7" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="E7" t="s">
+        <v>48</v>
+      </c>
+      <c r="F7" s="15"/>
+      <c r="I7" s="15" t="s">
+        <v>64</v>
+      </c>
+      <c r="J7" t="s">
+        <v>86</v>
+      </c>
+      <c r="K7" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>88</v>
+      </c>
+      <c r="B8" t="s">
+        <v>89</v>
+      </c>
+      <c r="C8" t="s">
+        <v>90</v>
+      </c>
+      <c r="D8" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="E8" t="s">
+        <v>48</v>
+      </c>
+      <c r="F8" s="15"/>
+      <c r="I8" s="15" t="s">
+        <v>64</v>
+      </c>
+      <c r="J8" t="s">
+        <v>91</v>
+      </c>
+      <c r="K8" t="s">
+        <v>113</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="21.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" s="13" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>71</v>
+      </c>
       <c r="B2" t="s">
-        <v>60</v>
-      </c>
-      <c r="C2" t="s">
-        <v>62</v>
-      </c>
-      <c r="D2" t="s">
-        <v>63</v>
-      </c>
-      <c r="E2" t="s">
-        <v>64</v>
-      </c>
-      <c r="F2" t="s">
-        <v>49</v>
-      </c>
-      <c r="G2" t="s">
-        <v>65</v>
-      </c>
-      <c r="J2" t="s">
-        <v>66</v>
-      </c>
-      <c r="L2" s="12" t="s">
-        <v>67</v>
-      </c>
-      <c r="M2" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>68</v>
+        <v>76</v>
       </c>
       <c r="B3" t="s">
-        <v>69</v>
-      </c>
-      <c r="C3" t="s">
-        <v>70</v>
-      </c>
-      <c r="D3" t="s">
-        <v>71</v>
-      </c>
-      <c r="E3" t="s">
-        <v>72</v>
-      </c>
-      <c r="F3" t="s">
-        <v>49</v>
-      </c>
-      <c r="G3" t="s">
-        <v>65</v>
-      </c>
-      <c r="J3" t="s">
-        <v>73</v>
-      </c>
-      <c r="L3" s="14">
-        <v>43742</v>
-      </c>
-      <c r="M3" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>74</v>
+        <v>80</v>
       </c>
       <c r="B4" t="s">
-        <v>75</v>
-      </c>
-      <c r="C4" t="s">
-        <v>76</v>
-      </c>
-      <c r="D4" t="s">
-        <v>63</v>
-      </c>
-      <c r="E4" t="s">
-        <v>77</v>
-      </c>
-      <c r="F4" t="s">
-        <v>49</v>
-      </c>
-      <c r="G4" t="s">
-        <v>65</v>
-      </c>
-      <c r="J4" t="s">
-        <v>78</v>
-      </c>
-      <c r="L4" t="s">
-        <v>79</v>
-      </c>
-      <c r="M4" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>80</v>
-      </c>
+        <v>116</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>81</v>
-      </c>
-      <c r="C5" t="s">
-        <v>82</v>
-      </c>
-      <c r="D5" t="s">
-        <v>63</v>
-      </c>
-      <c r="E5" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
         <v>83</v>
       </c>
-      <c r="F5" t="s">
-        <v>49</v>
-      </c>
-      <c r="G5" t="s">
-        <v>65</v>
-      </c>
-      <c r="J5" t="s">
-        <v>78</v>
-      </c>
-      <c r="L5" t="s">
-        <v>84</v>
-      </c>
-      <c r="M5" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>85</v>
-      </c>
-      <c r="B6" t="s">
-        <v>86</v>
-      </c>
-      <c r="C6" t="s">
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
         <v>87</v>
       </c>
-      <c r="D6" t="s">
-        <v>63</v>
-      </c>
-      <c r="E6" t="s">
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
         <v>88</v>
-      </c>
-      <c r="F6" t="s">
-        <v>49</v>
-      </c>
-      <c r="G6" t="s">
-        <v>65</v>
-      </c>
-      <c r="J6" t="s">
-        <v>78</v>
-      </c>
-      <c r="L6" t="s">
-        <v>89</v>
-      </c>
-      <c r="M6" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>94</v>
-      </c>
-      <c r="B7" t="s">
-        <v>90</v>
-      </c>
-      <c r="C7" t="s">
-        <v>91</v>
-      </c>
-      <c r="D7" t="s">
-        <v>63</v>
-      </c>
-      <c r="E7" t="s">
-        <v>92</v>
-      </c>
-      <c r="F7" t="s">
-        <v>49</v>
-      </c>
-      <c r="G7" t="s">
-        <v>65</v>
-      </c>
-      <c r="J7" t="s">
-        <v>66</v>
-      </c>
-      <c r="L7" t="s">
-        <v>93</v>
-      </c>
-      <c r="M7" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>95</v>
-      </c>
-      <c r="B8" t="s">
-        <v>96</v>
-      </c>
-      <c r="C8" t="s">
-        <v>97</v>
-      </c>
-      <c r="D8" t="s">
-        <v>63</v>
-      </c>
-      <c r="E8" t="s">
-        <v>98</v>
-      </c>
-      <c r="F8" t="s">
-        <v>49</v>
-      </c>
-      <c r="G8" t="s">
-        <v>65</v>
-      </c>
-      <c r="J8" t="s">
-        <v>66</v>
-      </c>
-      <c r="L8" t="s">
-        <v>99</v>
-      </c>
-      <c r="M8" t="s">
-        <v>65</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
jn: revisión de tipos de variables, ejemplos y definiciones
</commit_message>
<xml_diff>
--- a/04_Entregable 2/previo/metadatos y diccionario_AG.xlsx
+++ b/04_Entregable 2/previo/metadatos y diccionario_AG.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MAG\personal\consultorías\wcs\04_Entregable 2\previo\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Disco_F\!!Personal\Mio\1_WCS 2024\wcs\04_Entregable 2\previo\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28770" windowHeight="11385" firstSheet="2" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28770" windowHeight="11385" firstSheet="1" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Metadatos generales" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="120">
   <si>
     <t>Elemento</t>
   </si>
@@ -223,9 +223,6 @@
     <t>Código alfanumérico de entre 14 y 15 caractéres</t>
   </si>
   <si>
-    <t>variable de clasificación</t>
-  </si>
-  <si>
     <t>24281201901783</t>
   </si>
   <si>
@@ -241,9 +238,6 @@
     <t>date</t>
   </si>
   <si>
-    <t>variable temporal</t>
-  </si>
-  <si>
     <t>Provincia</t>
   </si>
   <si>
@@ -253,9 +247,6 @@
     <t>Provincia donde se ingresa el juicio</t>
   </si>
   <si>
-    <t>variable de ubicación</t>
-  </si>
-  <si>
     <t>SANTA ELENA</t>
   </si>
   <si>
@@ -386,6 +377,18 @@
   </si>
   <si>
     <t>TRIBUNAL PENAL</t>
+  </si>
+  <si>
+    <t>Identificación</t>
+  </si>
+  <si>
+    <t>Temporalidad</t>
+  </si>
+  <si>
+    <t>Localización</t>
+  </si>
+  <si>
+    <t>Transacción</t>
   </si>
 </sst>
 </file>
@@ -860,7 +863,7 @@
   <dimension ref="A2:C19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -911,7 +914,7 @@
         <v>30</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="30" x14ac:dyDescent="0.25">
@@ -1083,64 +1086,64 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="B1" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="B2" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="B3" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="B4" t="s">
+        <v>102</v>
+      </c>
+      <c r="C4" t="s">
+        <v>103</v>
+      </c>
+      <c r="D4" t="s">
+        <v>104</v>
+      </c>
+      <c r="E4" t="s">
         <v>105</v>
-      </c>
-      <c r="C4" t="s">
-        <v>106</v>
-      </c>
-      <c r="D4" t="s">
-        <v>107</v>
-      </c>
-      <c r="E4" t="s">
-        <v>108</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="B5" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="B6" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="B7" s="14">
         <v>45535</v>
@@ -1148,7 +1151,7 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
     </row>
   </sheetData>
@@ -1160,8 +1163,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A8"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1237,24 +1240,24 @@
         <v>63</v>
       </c>
       <c r="I2" s="15" t="s">
-        <v>52</v>
+        <v>116</v>
       </c>
       <c r="J2" s="12" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>65</v>
+      </c>
+      <c r="B3" t="s">
         <v>66</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>67</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" s="15" t="s">
         <v>68</v>
-      </c>
-      <c r="D3" s="15" t="s">
-        <v>69</v>
       </c>
       <c r="E3" t="s">
         <v>48</v>
@@ -1263,10 +1266,10 @@
         <v>48</v>
       </c>
       <c r="H3" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="I3" s="15" t="s">
-        <v>70</v>
+        <v>117</v>
       </c>
       <c r="J3" s="14">
         <v>43742</v>
@@ -1274,13 +1277,13 @@
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>69</v>
+      </c>
+      <c r="B4" t="s">
+        <v>70</v>
+      </c>
+      <c r="C4" t="s">
         <v>71</v>
-      </c>
-      <c r="B4" t="s">
-        <v>72</v>
-      </c>
-      <c r="C4" t="s">
-        <v>73</v>
       </c>
       <c r="D4" s="15" t="s">
         <v>62</v>
@@ -1289,27 +1292,27 @@
         <v>48</v>
       </c>
       <c r="F4" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="H4" t="s">
         <v>51</v>
       </c>
       <c r="I4" s="15" t="s">
-        <v>74</v>
+        <v>118</v>
       </c>
       <c r="J4" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="B5" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="C5" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="D5" s="15" t="s">
         <v>62</v>
@@ -1318,30 +1321,30 @@
         <v>48</v>
       </c>
       <c r="F5" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="G5" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="H5" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="I5" s="15" t="s">
-        <v>74</v>
+        <v>118</v>
       </c>
       <c r="J5" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="B6" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="C6" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="D6" s="15" t="s">
         <v>62</v>
@@ -1351,24 +1354,24 @@
       </c>
       <c r="F6" s="15"/>
       <c r="I6" s="15" t="s">
-        <v>74</v>
+        <v>6</v>
       </c>
       <c r="J6" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="K6" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="B7" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="C7" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="D7" s="15" t="s">
         <v>62</v>
@@ -1378,24 +1381,24 @@
       </c>
       <c r="F7" s="15"/>
       <c r="I7" s="15" t="s">
-        <v>64</v>
+        <v>119</v>
       </c>
       <c r="J7" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="K7" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="B8" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="C8" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="D8" s="15" t="s">
         <v>62</v>
@@ -1405,13 +1408,13 @@
       </c>
       <c r="F8" s="15"/>
       <c r="I8" s="15" t="s">
-        <v>64</v>
+        <v>6</v>
       </c>
       <c r="J8" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="K8" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
     </row>
   </sheetData>
@@ -1438,56 +1441,56 @@
         <v>13</v>
       </c>
       <c r="B1" s="13" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B2" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="B3" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="B4" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
AG: primeros diccionarios de variables realizados
</commit_message>
<xml_diff>
--- a/04_Entregable 2/previo/metadatos y diccionario_AG.xlsx
+++ b/04_Entregable 2/previo/metadatos y diccionario_AG.xlsx
@@ -9,14 +9,19 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28770" windowHeight="11385" firstSheet="2" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28770" windowHeight="11385"/>
   </bookViews>
   <sheets>
-    <sheet name="Metadatos generales" sheetId="1" r:id="rId1"/>
-    <sheet name="Hoja2" sheetId="2" r:id="rId2"/>
-    <sheet name="02_1_general" sheetId="4" r:id="rId3"/>
-    <sheet name="02_1_diccionario" sheetId="3" r:id="rId4"/>
-    <sheet name="02_1_dominios" sheetId="5" r:id="rId5"/>
+    <sheet name="04_1_diccionario" sheetId="10" r:id="rId1"/>
+    <sheet name="04_1_general" sheetId="11" r:id="rId2"/>
+    <sheet name="02_3_diccionario" sheetId="9" r:id="rId3"/>
+    <sheet name="02_3_general" sheetId="8" r:id="rId4"/>
+    <sheet name="02_2_general" sheetId="6" r:id="rId5"/>
+    <sheet name="02_2_diccionario" sheetId="7" r:id="rId6"/>
+    <sheet name="Metadatos generales" sheetId="1" r:id="rId7"/>
+    <sheet name="Hoja2" sheetId="2" r:id="rId8"/>
+    <sheet name="02_1_general" sheetId="4" r:id="rId9"/>
+    <sheet name="02_1_diccionario" sheetId="3" r:id="rId10"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -28,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="496" uniqueCount="192">
   <si>
     <t>Elemento</t>
   </si>
@@ -211,57 +216,30 @@
     <t>IDJUICIO</t>
   </si>
   <si>
-    <t>Identificador del juicio</t>
-  </si>
-  <si>
     <t>Identificador asignado al juicio</t>
   </si>
   <si>
-    <t>character</t>
-  </si>
-  <si>
     <t>Código alfanumérico de entre 14 y 15 caractéres</t>
   </si>
   <si>
-    <t>variable de clasificación</t>
-  </si>
-  <si>
     <t>24281201901783</t>
   </si>
   <si>
-    <t>Fecha de ingreso</t>
-  </si>
-  <si>
     <t>FECHA INGRESO</t>
   </si>
   <si>
     <t>Fecha de ingreso del juicio</t>
   </si>
   <si>
-    <t>date</t>
-  </si>
-  <si>
-    <t>variable temporal</t>
-  </si>
-  <si>
-    <t>Provincia</t>
-  </si>
-  <si>
     <t>PROVINCIA</t>
   </si>
   <si>
     <t>Provincia donde se ingresa el juicio</t>
   </si>
   <si>
-    <t>variable de ubicación</t>
-  </si>
-  <si>
     <t>SANTA ELENA</t>
   </si>
   <si>
-    <t>Cantón</t>
-  </si>
-  <si>
     <t>CANTON</t>
   </si>
   <si>
@@ -271,9 +249,6 @@
     <t>LA LIBERTAD</t>
   </si>
   <si>
-    <t>Instancia</t>
-  </si>
-  <si>
     <t>INSTANCIA</t>
   </si>
   <si>
@@ -292,12 +267,6 @@
     <t>247 DELITOS CONTRA LA FLORA Y FAUNA SILVESTRES</t>
   </si>
   <si>
-    <t>Delito</t>
-  </si>
-  <si>
-    <t>Estado causa</t>
-  </si>
-  <si>
     <t>ESTADO CAUSA</t>
   </si>
   <si>
@@ -373,19 +342,274 @@
     <t>VALORES DIFERENTES A LOS PRESENTES EN LA BASE</t>
   </si>
   <si>
-    <t>Valores</t>
-  </si>
-  <si>
-    <t>DPA por año</t>
-  </si>
-  <si>
-    <t>CORTE NACIONAL</t>
-  </si>
-  <si>
-    <t>SALA DE CORTE PROVINCIAL</t>
-  </si>
-  <si>
-    <t>TRIBUNAL PENAL</t>
+    <t>Cadena</t>
+  </si>
+  <si>
+    <t>Fecha y Hora</t>
+  </si>
+  <si>
+    <t>Categórica</t>
+  </si>
+  <si>
+    <t>Identificación</t>
+  </si>
+  <si>
+    <t>Temporalidad</t>
+  </si>
+  <si>
+    <t>Localización</t>
+  </si>
+  <si>
+    <t>Transacción o Evento</t>
+  </si>
+  <si>
+    <t>Causas Resueltas</t>
+  </si>
+  <si>
+    <t>CAUSAS RESUELTAS</t>
+  </si>
+  <si>
+    <t>B6:J202</t>
+  </si>
+  <si>
+    <t>FECHA PROVIDENCIA</t>
+  </si>
+  <si>
+    <t>Fecha de providencia del juicio</t>
+  </si>
+  <si>
+    <t>PROVIDENCIA</t>
+  </si>
+  <si>
+    <t>Resolución del juicio</t>
+  </si>
+  <si>
+    <t>Expresión que describe la resolución del juicio</t>
+  </si>
+  <si>
+    <t>SENTENCIA CONDENATORIA</t>
+  </si>
+  <si>
+    <t>DETERMINAR SI SE PUEDE ENGLOBAR EN CATEGORÍAS</t>
+  </si>
+  <si>
+    <t>FORMAS DE TERMINACIÓN</t>
+  </si>
+  <si>
+    <t>Forma de terminación del juicio</t>
+  </si>
+  <si>
+    <t>Expresión que describe la forma de terminación del juicio</t>
+  </si>
+  <si>
+    <t>CAUSAS RESUELTAS , "RAZON DE EJECUTORIA"</t>
+  </si>
+  <si>
+    <t>B6:I114</t>
+  </si>
+  <si>
+    <t>Causas Razón de ejecutoría</t>
+  </si>
+  <si>
+    <t>FECHA_PROVIDENCIAACTIVIDAD</t>
+  </si>
+  <si>
+    <t>NOMBRE_PROVIDENCIAACTIVIDAD</t>
+  </si>
+  <si>
+    <t>Fecha de providencia de actividad</t>
+  </si>
+  <si>
+    <t>Nombre de providencia de actividad</t>
+  </si>
+  <si>
+    <t>RAZON DE EJECUTORIA</t>
+  </si>
+  <si>
+    <t>Consolidado 2020_Retenciones y Rescates_Zonales</t>
+  </si>
+  <si>
+    <t>xlsm</t>
+  </si>
+  <si>
+    <t>Rescate</t>
+  </si>
+  <si>
+    <t>RESPONSABLE:</t>
+  </si>
+  <si>
+    <t>MIRIAM MOPOSITA</t>
+  </si>
+  <si>
+    <t>FECHA:</t>
+  </si>
+  <si>
+    <t>ENERO-JUNIO 2020</t>
+  </si>
+  <si>
+    <t>A7:Y733</t>
+  </si>
+  <si>
+    <t>Ministerio del Ambiente y Agua</t>
+  </si>
+  <si>
+    <t>Código Acta</t>
+  </si>
+  <si>
+    <t>Fecha del rescate</t>
+  </si>
+  <si>
+    <t>Hora de rescate</t>
+  </si>
+  <si>
+    <t>X</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>Nombres</t>
+  </si>
+  <si>
+    <t>Apellidos</t>
+  </si>
+  <si>
+    <t>Cédula o Pasaporte</t>
+  </si>
+  <si>
+    <t>Filiación Institucional</t>
+  </si>
+  <si>
+    <t>Forma de aviso</t>
+  </si>
+  <si>
+    <t>Reino</t>
+  </si>
+  <si>
+    <t>Clase</t>
+  </si>
+  <si>
+    <t>Nombre científico</t>
+  </si>
+  <si>
+    <t>Nombre Común</t>
+  </si>
+  <si>
+    <t>Machos</t>
+  </si>
+  <si>
+    <t>Hembras</t>
+  </si>
+  <si>
+    <t>Indet.</t>
+  </si>
+  <si>
+    <t>Etapa de vida</t>
+  </si>
+  <si>
+    <t>Estado Físico</t>
+  </si>
+  <si>
+    <t>Razón social del Destino</t>
+  </si>
+  <si>
+    <t>Fecha de Entrega</t>
+  </si>
+  <si>
+    <t>Destino final</t>
+  </si>
+  <si>
+    <t>Acta Desntino Final</t>
+  </si>
+  <si>
+    <t>Código de acta del registro de rescate</t>
+  </si>
+  <si>
+    <t>Hora del rescate</t>
+  </si>
+  <si>
+    <t>Coordenada UTM X</t>
+  </si>
+  <si>
+    <t>Coordenada UTM Y</t>
+  </si>
+  <si>
+    <t>Nombres del rescatista</t>
+  </si>
+  <si>
+    <t>Apellidos del rescatista</t>
+  </si>
+  <si>
+    <t>Cédula o Pasaporte del Rescatista</t>
+  </si>
+  <si>
+    <t>Institución a la que pertenece el rescatista</t>
+  </si>
+  <si>
+    <t>Forma de aviso para dar paso al rescate</t>
+  </si>
+  <si>
+    <t>Reino al que pertenece la vida silvestre rescatada</t>
+  </si>
+  <si>
+    <t>Clase a la que pertenece la vida silvestre rescatada</t>
+  </si>
+  <si>
+    <t>Nombre científico de la vida silvestre rescatada</t>
+  </si>
+  <si>
+    <t>Nombre común de la vida silvestre rescatada</t>
+  </si>
+  <si>
+    <t>Número de individuos machos rescatados</t>
+  </si>
+  <si>
+    <t>Número de individuos hembras rescatados</t>
+  </si>
+  <si>
+    <t>Número de individuos de sexo indeterminados rescatados</t>
+  </si>
+  <si>
+    <t>Etapa de vida de la vida silvestre rescatada</t>
+  </si>
+  <si>
+    <t>Estado físico de la vida silvestre rescatada</t>
+  </si>
+  <si>
+    <t>Razón social del lugar de destino de la vida silvestre rescatada</t>
+  </si>
+  <si>
+    <t>Nombres del responsable de recepción de la vida silvestre rescatada en el lugar de destino</t>
+  </si>
+  <si>
+    <t>Apellidos del responsable de recepción de la vida silvestre rescatada en el lugar de destino</t>
+  </si>
+  <si>
+    <t>Fecha de entrega de la vida silvestre rescatada al lugar de destino</t>
+  </si>
+  <si>
+    <t>Destino final de la vida silvestre</t>
+  </si>
+  <si>
+    <t>Código de acta del destino final de la vida silvestre rescatada</t>
+  </si>
+  <si>
+    <t>Numérica</t>
+  </si>
+  <si>
+    <t>Registro de Rescate</t>
+  </si>
+  <si>
+    <t>Coordenadas UTM</t>
+  </si>
+  <si>
+    <t>Datos del Rescatista</t>
+  </si>
+  <si>
+    <t>Datos de la Vida Silvestre Rescatada</t>
+  </si>
+  <si>
+    <t>Medios de Conservación y Manejo Ex Situ</t>
   </si>
 </sst>
 </file>
@@ -468,7 +692,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -505,10 +729,14 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFill="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -789,6 +1017,1606 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J26"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="28.5703125" style="19" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.42578125" style="19" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.7109375" style="19" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.28515625" style="19" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.42578125" style="19" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.5703125" style="19" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.5703125" style="19" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="22.28515625" style="19" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.85546875" style="19" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.7109375" style="19" bestFit="1" customWidth="1"/>
+    <col min="11" max="16384" width="11.42578125" style="19"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1" s="18" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="D1" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="F1" s="18" t="s">
+        <v>19</v>
+      </c>
+      <c r="G1" s="18" t="s">
+        <v>20</v>
+      </c>
+      <c r="H1" s="18" t="s">
+        <v>21</v>
+      </c>
+      <c r="I1" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="J1" s="18" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" s="19" t="s">
+        <v>139</v>
+      </c>
+      <c r="B2" s="19" t="s">
+        <v>162</v>
+      </c>
+      <c r="C2" s="19" t="s">
+        <v>102</v>
+      </c>
+      <c r="D2" s="19" t="s">
+        <v>48</v>
+      </c>
+      <c r="E2" s="19" t="s">
+        <v>48</v>
+      </c>
+      <c r="F2" s="19" t="s">
+        <v>187</v>
+      </c>
+      <c r="I2" s="20"/>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" s="19" t="s">
+        <v>140</v>
+      </c>
+      <c r="B3" s="19" t="s">
+        <v>140</v>
+      </c>
+      <c r="C3" s="19" t="s">
+        <v>103</v>
+      </c>
+      <c r="D3" s="19" t="s">
+        <v>48</v>
+      </c>
+      <c r="E3" s="19" t="s">
+        <v>48</v>
+      </c>
+      <c r="F3" s="19" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" s="19" t="s">
+        <v>141</v>
+      </c>
+      <c r="B4" s="19" t="s">
+        <v>163</v>
+      </c>
+      <c r="C4" s="19" t="s">
+        <v>103</v>
+      </c>
+      <c r="D4" s="19" t="s">
+        <v>48</v>
+      </c>
+      <c r="E4" s="19" t="s">
+        <v>48</v>
+      </c>
+      <c r="F4" s="19" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" s="19" t="s">
+        <v>142</v>
+      </c>
+      <c r="B5" s="19" t="s">
+        <v>164</v>
+      </c>
+      <c r="C5" s="19" t="s">
+        <v>186</v>
+      </c>
+      <c r="D5" s="19" t="s">
+        <v>48</v>
+      </c>
+      <c r="E5" s="19" t="s">
+        <v>48</v>
+      </c>
+      <c r="F5" s="19" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" s="19" t="s">
+        <v>143</v>
+      </c>
+      <c r="B6" s="19" t="s">
+        <v>165</v>
+      </c>
+      <c r="C6" s="19" t="s">
+        <v>186</v>
+      </c>
+      <c r="D6" s="19" t="s">
+        <v>48</v>
+      </c>
+      <c r="E6" s="19" t="s">
+        <v>48</v>
+      </c>
+      <c r="F6" s="19" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" s="15" t="s">
+        <v>144</v>
+      </c>
+      <c r="B7" s="19" t="s">
+        <v>166</v>
+      </c>
+      <c r="C7" s="19" t="s">
+        <v>102</v>
+      </c>
+      <c r="D7" s="19" t="s">
+        <v>48</v>
+      </c>
+      <c r="E7" s="19" t="s">
+        <v>48</v>
+      </c>
+      <c r="F7" s="19" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" s="15" t="s">
+        <v>145</v>
+      </c>
+      <c r="B8" s="19" t="s">
+        <v>167</v>
+      </c>
+      <c r="C8" s="19" t="s">
+        <v>102</v>
+      </c>
+      <c r="D8" s="19" t="s">
+        <v>48</v>
+      </c>
+      <c r="E8" s="19" t="s">
+        <v>48</v>
+      </c>
+      <c r="F8" s="19" t="s">
+        <v>189</v>
+      </c>
+      <c r="I8" s="21"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" s="19" t="s">
+        <v>146</v>
+      </c>
+      <c r="B9" s="19" t="s">
+        <v>168</v>
+      </c>
+      <c r="C9" s="19" t="s">
+        <v>102</v>
+      </c>
+      <c r="D9" s="19" t="s">
+        <v>48</v>
+      </c>
+      <c r="E9" s="19" t="s">
+        <v>48</v>
+      </c>
+      <c r="F9" s="19" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10" s="19" t="s">
+        <v>147</v>
+      </c>
+      <c r="B10" s="19" t="s">
+        <v>169</v>
+      </c>
+      <c r="C10" s="19" t="s">
+        <v>104</v>
+      </c>
+      <c r="D10" s="19" t="s">
+        <v>48</v>
+      </c>
+      <c r="F10" s="19" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11" s="19" t="s">
+        <v>148</v>
+      </c>
+      <c r="B11" s="19" t="s">
+        <v>170</v>
+      </c>
+      <c r="C11" s="19" t="s">
+        <v>104</v>
+      </c>
+      <c r="D11" s="19" t="s">
+        <v>48</v>
+      </c>
+      <c r="E11" s="19" t="s">
+        <v>48</v>
+      </c>
+      <c r="F11" s="19" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12" s="19" t="s">
+        <v>149</v>
+      </c>
+      <c r="B12" s="19" t="s">
+        <v>171</v>
+      </c>
+      <c r="C12" s="19" t="s">
+        <v>104</v>
+      </c>
+      <c r="D12" s="19" t="s">
+        <v>48</v>
+      </c>
+      <c r="F12" s="19" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13" s="19" t="s">
+        <v>150</v>
+      </c>
+      <c r="B13" s="19" t="s">
+        <v>172</v>
+      </c>
+      <c r="C13" s="19" t="s">
+        <v>104</v>
+      </c>
+      <c r="D13" s="19" t="s">
+        <v>48</v>
+      </c>
+      <c r="F13" s="19" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A14" s="19" t="s">
+        <v>151</v>
+      </c>
+      <c r="B14" s="19" t="s">
+        <v>173</v>
+      </c>
+      <c r="C14" s="19" t="s">
+        <v>104</v>
+      </c>
+      <c r="D14" s="19" t="s">
+        <v>48</v>
+      </c>
+      <c r="F14" s="19" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A15" s="19" t="s">
+        <v>152</v>
+      </c>
+      <c r="B15" s="19" t="s">
+        <v>174</v>
+      </c>
+      <c r="C15" s="19" t="s">
+        <v>102</v>
+      </c>
+      <c r="D15" s="19" t="s">
+        <v>48</v>
+      </c>
+      <c r="E15" s="19" t="s">
+        <v>48</v>
+      </c>
+      <c r="F15" s="19" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A16" s="19" t="s">
+        <v>153</v>
+      </c>
+      <c r="B16" s="19" t="s">
+        <v>175</v>
+      </c>
+      <c r="C16" s="19" t="s">
+        <v>186</v>
+      </c>
+      <c r="D16" s="19" t="s">
+        <v>48</v>
+      </c>
+      <c r="F16" s="19" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" s="19" t="s">
+        <v>154</v>
+      </c>
+      <c r="B17" s="19" t="s">
+        <v>176</v>
+      </c>
+      <c r="C17" s="19" t="s">
+        <v>186</v>
+      </c>
+      <c r="D17" s="19" t="s">
+        <v>48</v>
+      </c>
+      <c r="E17" s="19" t="s">
+        <v>48</v>
+      </c>
+      <c r="F17" s="19" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" s="19" t="s">
+        <v>155</v>
+      </c>
+      <c r="B18" s="19" t="s">
+        <v>177</v>
+      </c>
+      <c r="C18" s="19" t="s">
+        <v>186</v>
+      </c>
+      <c r="D18" s="19" t="s">
+        <v>48</v>
+      </c>
+      <c r="E18" s="19" t="s">
+        <v>48</v>
+      </c>
+      <c r="F18" s="19" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" s="17" t="s">
+        <v>156</v>
+      </c>
+      <c r="B19" s="19" t="s">
+        <v>178</v>
+      </c>
+      <c r="C19" s="19" t="s">
+        <v>104</v>
+      </c>
+      <c r="D19" s="19" t="s">
+        <v>48</v>
+      </c>
+      <c r="E19" s="19" t="s">
+        <v>48</v>
+      </c>
+      <c r="F19" s="19" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" s="17" t="s">
+        <v>157</v>
+      </c>
+      <c r="B20" s="19" t="s">
+        <v>179</v>
+      </c>
+      <c r="C20" s="19" t="s">
+        <v>104</v>
+      </c>
+      <c r="D20" s="19" t="s">
+        <v>48</v>
+      </c>
+      <c r="E20" s="19" t="s">
+        <v>48</v>
+      </c>
+      <c r="F20" s="19" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" s="19" t="s">
+        <v>158</v>
+      </c>
+      <c r="B21" s="19" t="s">
+        <v>180</v>
+      </c>
+      <c r="C21" s="19" t="s">
+        <v>102</v>
+      </c>
+      <c r="D21" s="19" t="s">
+        <v>48</v>
+      </c>
+      <c r="E21" s="19" t="s">
+        <v>48</v>
+      </c>
+      <c r="F21" s="19" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" s="15" t="s">
+        <v>144</v>
+      </c>
+      <c r="B22" s="19" t="s">
+        <v>181</v>
+      </c>
+      <c r="C22" s="19" t="s">
+        <v>102</v>
+      </c>
+      <c r="D22" s="19" t="s">
+        <v>48</v>
+      </c>
+      <c r="E22" s="19" t="s">
+        <v>48</v>
+      </c>
+      <c r="F22" s="19" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" s="15" t="s">
+        <v>145</v>
+      </c>
+      <c r="B23" s="19" t="s">
+        <v>182</v>
+      </c>
+      <c r="C23" s="19" t="s">
+        <v>102</v>
+      </c>
+      <c r="D23" s="19" t="s">
+        <v>48</v>
+      </c>
+      <c r="E23" s="19" t="s">
+        <v>48</v>
+      </c>
+      <c r="F23" s="19" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" s="19" t="s">
+        <v>159</v>
+      </c>
+      <c r="B24" s="19" t="s">
+        <v>183</v>
+      </c>
+      <c r="C24" s="19" t="s">
+        <v>103</v>
+      </c>
+      <c r="D24" s="19" t="s">
+        <v>48</v>
+      </c>
+      <c r="E24" s="19" t="s">
+        <v>48</v>
+      </c>
+      <c r="F24" s="19" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" s="19" t="s">
+        <v>160</v>
+      </c>
+      <c r="B25" s="19" t="s">
+        <v>184</v>
+      </c>
+      <c r="C25" s="19" t="s">
+        <v>104</v>
+      </c>
+      <c r="D25" s="19" t="s">
+        <v>48</v>
+      </c>
+      <c r="F25" s="19" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26" s="19" t="s">
+        <v>161</v>
+      </c>
+      <c r="B26" s="19" t="s">
+        <v>185</v>
+      </c>
+      <c r="C26" s="19" t="s">
+        <v>102</v>
+      </c>
+      <c r="D26" s="19" t="s">
+        <v>48</v>
+      </c>
+      <c r="E26" s="19" t="s">
+        <v>48</v>
+      </c>
+      <c r="F26" s="19" t="s">
+        <v>191</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:B1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="21.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.7109375" style="19" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="22.28515625" style="19" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="D1" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="F1" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="G1" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="H1" s="18" t="s">
+        <v>21</v>
+      </c>
+      <c r="I1" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="J1" s="13" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>59</v>
+      </c>
+      <c r="B2" t="s">
+        <v>60</v>
+      </c>
+      <c r="C2" s="19" t="s">
+        <v>102</v>
+      </c>
+      <c r="D2" t="s">
+        <v>48</v>
+      </c>
+      <c r="E2" t="s">
+        <v>48</v>
+      </c>
+      <c r="G2" s="15" t="s">
+        <v>61</v>
+      </c>
+      <c r="H2" s="19" t="s">
+        <v>105</v>
+      </c>
+      <c r="I2" s="12" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>63</v>
+      </c>
+      <c r="B3" t="s">
+        <v>64</v>
+      </c>
+      <c r="C3" s="19" t="s">
+        <v>103</v>
+      </c>
+      <c r="D3" t="s">
+        <v>48</v>
+      </c>
+      <c r="E3" t="s">
+        <v>48</v>
+      </c>
+      <c r="G3" t="s">
+        <v>100</v>
+      </c>
+      <c r="H3" s="19" t="s">
+        <v>106</v>
+      </c>
+      <c r="I3" s="14">
+        <v>43742</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>65</v>
+      </c>
+      <c r="B4" t="s">
+        <v>66</v>
+      </c>
+      <c r="C4" s="19" t="s">
+        <v>104</v>
+      </c>
+      <c r="D4" t="s">
+        <v>48</v>
+      </c>
+      <c r="E4" t="s">
+        <v>82</v>
+      </c>
+      <c r="G4" t="s">
+        <v>51</v>
+      </c>
+      <c r="H4" s="19" t="s">
+        <v>107</v>
+      </c>
+      <c r="I4" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>68</v>
+      </c>
+      <c r="B5" t="s">
+        <v>69</v>
+      </c>
+      <c r="C5" s="19" t="s">
+        <v>104</v>
+      </c>
+      <c r="D5" t="s">
+        <v>48</v>
+      </c>
+      <c r="E5" t="s">
+        <v>82</v>
+      </c>
+      <c r="F5" t="s">
+        <v>65</v>
+      </c>
+      <c r="G5" t="s">
+        <v>80</v>
+      </c>
+      <c r="H5" s="19" t="s">
+        <v>107</v>
+      </c>
+      <c r="I5" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>71</v>
+      </c>
+      <c r="B6" t="s">
+        <v>72</v>
+      </c>
+      <c r="C6" s="19" t="s">
+        <v>104</v>
+      </c>
+      <c r="D6" t="s">
+        <v>48</v>
+      </c>
+      <c r="E6" s="15"/>
+      <c r="H6" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="I6" t="s">
+        <v>73</v>
+      </c>
+      <c r="J6" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>74</v>
+      </c>
+      <c r="B7" t="s">
+        <v>75</v>
+      </c>
+      <c r="C7" s="19" t="s">
+        <v>104</v>
+      </c>
+      <c r="D7" t="s">
+        <v>48</v>
+      </c>
+      <c r="E7" s="15"/>
+      <c r="H7" s="19" t="s">
+        <v>108</v>
+      </c>
+      <c r="I7" t="s">
+        <v>76</v>
+      </c>
+      <c r="J7" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>77</v>
+      </c>
+      <c r="B8" t="s">
+        <v>78</v>
+      </c>
+      <c r="C8" s="19" t="s">
+        <v>104</v>
+      </c>
+      <c r="D8" t="s">
+        <v>48</v>
+      </c>
+      <c r="E8" s="15"/>
+      <c r="H8" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="I8" t="s">
+        <v>79</v>
+      </c>
+      <c r="J8" t="s">
+        <v>101</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="25.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>83</v>
+      </c>
+      <c r="B1" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>84</v>
+      </c>
+      <c r="B2" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>85</v>
+      </c>
+      <c r="B3" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>87</v>
+      </c>
+      <c r="B4" t="s">
+        <v>133</v>
+      </c>
+      <c r="C4" t="s">
+        <v>134</v>
+      </c>
+      <c r="D4" t="s">
+        <v>135</v>
+      </c>
+      <c r="E4" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>86</v>
+      </c>
+      <c r="B5" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>88</v>
+      </c>
+      <c r="B6" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>99</v>
+      </c>
+      <c r="B7" s="14"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>89</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="28.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.7109375" style="19" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="22.28515625" style="19" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="D1" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="F1" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="G1" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="H1" s="18" t="s">
+        <v>21</v>
+      </c>
+      <c r="I1" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="J1" s="13" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>59</v>
+      </c>
+      <c r="B2" t="s">
+        <v>60</v>
+      </c>
+      <c r="C2" s="19" t="s">
+        <v>102</v>
+      </c>
+      <c r="D2" t="s">
+        <v>48</v>
+      </c>
+      <c r="E2" t="s">
+        <v>48</v>
+      </c>
+      <c r="G2" s="15" t="s">
+        <v>61</v>
+      </c>
+      <c r="H2" s="19" t="s">
+        <v>105</v>
+      </c>
+      <c r="I2" s="12" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>65</v>
+      </c>
+      <c r="B3" t="s">
+        <v>66</v>
+      </c>
+      <c r="C3" s="19" t="s">
+        <v>104</v>
+      </c>
+      <c r="D3" t="s">
+        <v>48</v>
+      </c>
+      <c r="E3" t="s">
+        <v>82</v>
+      </c>
+      <c r="G3" t="s">
+        <v>51</v>
+      </c>
+      <c r="H3" s="19" t="s">
+        <v>107</v>
+      </c>
+      <c r="I3" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>68</v>
+      </c>
+      <c r="B4" t="s">
+        <v>69</v>
+      </c>
+      <c r="C4" s="19" t="s">
+        <v>104</v>
+      </c>
+      <c r="D4" t="s">
+        <v>48</v>
+      </c>
+      <c r="E4" t="s">
+        <v>82</v>
+      </c>
+      <c r="F4" t="s">
+        <v>65</v>
+      </c>
+      <c r="G4" t="s">
+        <v>80</v>
+      </c>
+      <c r="H4" s="19" t="s">
+        <v>107</v>
+      </c>
+      <c r="I4" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>71</v>
+      </c>
+      <c r="B5" t="s">
+        <v>72</v>
+      </c>
+      <c r="C5" s="19" t="s">
+        <v>104</v>
+      </c>
+      <c r="D5" t="s">
+        <v>48</v>
+      </c>
+      <c r="E5" s="15"/>
+      <c r="H5" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="I5" t="s">
+        <v>73</v>
+      </c>
+      <c r="J5" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>74</v>
+      </c>
+      <c r="B6" t="s">
+        <v>75</v>
+      </c>
+      <c r="C6" s="19" t="s">
+        <v>104</v>
+      </c>
+      <c r="D6" t="s">
+        <v>48</v>
+      </c>
+      <c r="E6" s="15"/>
+      <c r="H6" s="19" t="s">
+        <v>108</v>
+      </c>
+      <c r="I6" t="s">
+        <v>76</v>
+      </c>
+      <c r="J6" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>77</v>
+      </c>
+      <c r="B7" t="s">
+        <v>78</v>
+      </c>
+      <c r="C7" s="19" t="s">
+        <v>104</v>
+      </c>
+      <c r="D7" t="s">
+        <v>48</v>
+      </c>
+      <c r="E7" s="15"/>
+      <c r="H7" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="I7" t="s">
+        <v>79</v>
+      </c>
+      <c r="J7" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>125</v>
+      </c>
+      <c r="B8" t="s">
+        <v>127</v>
+      </c>
+      <c r="C8" s="19" t="s">
+        <v>103</v>
+      </c>
+      <c r="D8" t="s">
+        <v>48</v>
+      </c>
+      <c r="E8" t="s">
+        <v>48</v>
+      </c>
+      <c r="G8" t="s">
+        <v>100</v>
+      </c>
+      <c r="H8" s="19" t="s">
+        <v>106</v>
+      </c>
+      <c r="I8" s="14">
+        <v>44083</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>126</v>
+      </c>
+      <c r="B9" t="s">
+        <v>128</v>
+      </c>
+      <c r="C9" s="19" t="s">
+        <v>104</v>
+      </c>
+      <c r="D9" s="19" t="s">
+        <v>48</v>
+      </c>
+      <c r="E9" s="15"/>
+      <c r="G9" t="s">
+        <v>51</v>
+      </c>
+      <c r="H9" s="19" t="s">
+        <v>108</v>
+      </c>
+      <c r="I9" t="s">
+        <v>129</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="25.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>83</v>
+      </c>
+      <c r="B1" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>84</v>
+      </c>
+      <c r="B2" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>85</v>
+      </c>
+      <c r="B3" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>87</v>
+      </c>
+      <c r="B4" t="s">
+        <v>93</v>
+      </c>
+      <c r="C4" t="s">
+        <v>94</v>
+      </c>
+      <c r="D4" t="s">
+        <v>122</v>
+      </c>
+      <c r="E4" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>86</v>
+      </c>
+      <c r="B5" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>88</v>
+      </c>
+      <c r="B6" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>99</v>
+      </c>
+      <c r="B7" s="14">
+        <v>45535</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>89</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="25.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>83</v>
+      </c>
+      <c r="B1" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>84</v>
+      </c>
+      <c r="B2" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>85</v>
+      </c>
+      <c r="B3" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>87</v>
+      </c>
+      <c r="B4" t="s">
+        <v>93</v>
+      </c>
+      <c r="C4" t="s">
+        <v>94</v>
+      </c>
+      <c r="D4" t="s">
+        <v>110</v>
+      </c>
+      <c r="E4" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>86</v>
+      </c>
+      <c r="B5" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>88</v>
+      </c>
+      <c r="B6" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>99</v>
+      </c>
+      <c r="B7" s="14">
+        <v>45535</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>89</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:B1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="21.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.7109375" style="19" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="22.28515625" style="19" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="D1" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="F1" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="G1" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="H1" s="18" t="s">
+        <v>21</v>
+      </c>
+      <c r="I1" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="J1" s="13" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>59</v>
+      </c>
+      <c r="B2" t="s">
+        <v>60</v>
+      </c>
+      <c r="C2" s="19" t="s">
+        <v>102</v>
+      </c>
+      <c r="D2" t="s">
+        <v>48</v>
+      </c>
+      <c r="E2" t="s">
+        <v>48</v>
+      </c>
+      <c r="G2" s="15" t="s">
+        <v>61</v>
+      </c>
+      <c r="H2" s="19" t="s">
+        <v>105</v>
+      </c>
+      <c r="I2" s="12" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>112</v>
+      </c>
+      <c r="B3" t="s">
+        <v>113</v>
+      </c>
+      <c r="C3" s="19" t="s">
+        <v>103</v>
+      </c>
+      <c r="D3" t="s">
+        <v>48</v>
+      </c>
+      <c r="E3" t="s">
+        <v>48</v>
+      </c>
+      <c r="G3" t="s">
+        <v>100</v>
+      </c>
+      <c r="H3" s="19" t="s">
+        <v>106</v>
+      </c>
+      <c r="I3" s="14">
+        <v>43754</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>65</v>
+      </c>
+      <c r="B4" t="s">
+        <v>66</v>
+      </c>
+      <c r="C4" s="19" t="s">
+        <v>104</v>
+      </c>
+      <c r="D4" t="s">
+        <v>48</v>
+      </c>
+      <c r="E4" t="s">
+        <v>82</v>
+      </c>
+      <c r="G4" t="s">
+        <v>51</v>
+      </c>
+      <c r="H4" s="19" t="s">
+        <v>107</v>
+      </c>
+      <c r="I4" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>68</v>
+      </c>
+      <c r="B5" t="s">
+        <v>69</v>
+      </c>
+      <c r="C5" s="19" t="s">
+        <v>104</v>
+      </c>
+      <c r="D5" t="s">
+        <v>48</v>
+      </c>
+      <c r="E5" t="s">
+        <v>82</v>
+      </c>
+      <c r="F5" t="s">
+        <v>65</v>
+      </c>
+      <c r="G5" t="s">
+        <v>80</v>
+      </c>
+      <c r="H5" s="19" t="s">
+        <v>107</v>
+      </c>
+      <c r="I5" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>71</v>
+      </c>
+      <c r="B6" t="s">
+        <v>72</v>
+      </c>
+      <c r="C6" s="19" t="s">
+        <v>104</v>
+      </c>
+      <c r="D6" t="s">
+        <v>48</v>
+      </c>
+      <c r="E6" s="15"/>
+      <c r="H6" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="I6" t="s">
+        <v>73</v>
+      </c>
+      <c r="J6" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>74</v>
+      </c>
+      <c r="B7" t="s">
+        <v>75</v>
+      </c>
+      <c r="C7" s="19" t="s">
+        <v>104</v>
+      </c>
+      <c r="D7" t="s">
+        <v>48</v>
+      </c>
+      <c r="E7" s="15"/>
+      <c r="H7" s="19" t="s">
+        <v>108</v>
+      </c>
+      <c r="I7" t="s">
+        <v>76</v>
+      </c>
+      <c r="J7" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>77</v>
+      </c>
+      <c r="B8" t="s">
+        <v>78</v>
+      </c>
+      <c r="C8" s="19" t="s">
+        <v>104</v>
+      </c>
+      <c r="D8" t="s">
+        <v>48</v>
+      </c>
+      <c r="E8" s="15"/>
+      <c r="H8" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="I8" t="s">
+        <v>79</v>
+      </c>
+      <c r="J8" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>114</v>
+      </c>
+      <c r="B9" t="s">
+        <v>115</v>
+      </c>
+      <c r="C9" s="19" t="s">
+        <v>102</v>
+      </c>
+      <c r="D9" s="19" t="s">
+        <v>48</v>
+      </c>
+      <c r="G9" t="s">
+        <v>116</v>
+      </c>
+      <c r="H9" s="19" t="s">
+        <v>108</v>
+      </c>
+      <c r="I9" t="s">
+        <v>117</v>
+      </c>
+      <c r="J9" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>119</v>
+      </c>
+      <c r="B10" t="s">
+        <v>120</v>
+      </c>
+      <c r="C10" s="19" t="s">
+        <v>102</v>
+      </c>
+      <c r="D10" s="19" t="s">
+        <v>48</v>
+      </c>
+      <c r="G10" t="s">
+        <v>121</v>
+      </c>
+      <c r="H10" s="19" t="s">
+        <v>108</v>
+      </c>
+      <c r="I10" t="s">
+        <v>117</v>
+      </c>
+      <c r="J10" t="s">
+        <v>118</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:B7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -855,7 +2683,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:C19"/>
   <sheetViews>
@@ -911,7 +2739,7 @@
         <v>30</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>93</v>
+        <v>81</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="30" x14ac:dyDescent="0.25">
@@ -948,24 +2776,24 @@
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="17" t="s">
+      <c r="A9" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="B9" s="17" t="s">
+      <c r="B9" s="16" t="s">
         <v>34</v>
       </c>
-      <c r="C9" s="17" t="s">
+      <c r="C9" s="16" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A10" s="17" t="s">
+      <c r="A10" s="16" t="s">
         <v>19</v>
       </c>
-      <c r="B10" s="17" t="s">
+      <c r="B10" s="16" t="s">
         <v>35</v>
       </c>
-      <c r="C10" s="17" t="s">
+      <c r="C10" s="16" t="s">
         <v>50</v>
       </c>
     </row>
@@ -1068,7 +2896,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E8"/>
   <sheetViews>
@@ -1083,64 +2911,64 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>95</v>
+        <v>83</v>
       </c>
       <c r="B1" t="s">
-        <v>102</v>
+        <v>90</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>96</v>
+        <v>84</v>
       </c>
       <c r="B2" t="s">
-        <v>103</v>
+        <v>91</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>97</v>
+        <v>85</v>
       </c>
       <c r="B3" t="s">
-        <v>104</v>
+        <v>92</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>99</v>
+        <v>87</v>
       </c>
       <c r="B4" t="s">
-        <v>105</v>
+        <v>93</v>
       </c>
       <c r="C4" t="s">
-        <v>106</v>
+        <v>94</v>
       </c>
       <c r="D4" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="E4" t="s">
-        <v>108</v>
+        <v>96</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>98</v>
+        <v>86</v>
       </c>
       <c r="B5" t="s">
-        <v>109</v>
+        <v>97</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>100</v>
+        <v>88</v>
       </c>
       <c r="B6" t="s">
-        <v>110</v>
+        <v>98</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>111</v>
+        <v>99</v>
       </c>
       <c r="B7" s="14">
         <v>45535</v>
@@ -1148,350 +2976,10 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>101</v>
+        <v>89</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K8"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A8"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="21.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="28.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.7109375" style="15" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="22.28515625" style="15" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="16.7109375" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="B1" s="13" t="s">
-        <v>13</v>
-      </c>
-      <c r="C1" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="D1" s="16" t="s">
-        <v>15</v>
-      </c>
-      <c r="E1" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="F1" s="13" t="s">
-        <v>18</v>
-      </c>
-      <c r="G1" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="H1" s="13" t="s">
-        <v>20</v>
-      </c>
-      <c r="I1" s="16" t="s">
-        <v>21</v>
-      </c>
-      <c r="J1" s="13" t="s">
-        <v>23</v>
-      </c>
-      <c r="K1" s="13" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>60</v>
-      </c>
-      <c r="B2" t="s">
-        <v>59</v>
-      </c>
-      <c r="C2" t="s">
-        <v>61</v>
-      </c>
-      <c r="D2" s="15" t="s">
-        <v>62</v>
-      </c>
-      <c r="E2" t="s">
-        <v>48</v>
-      </c>
-      <c r="F2" t="s">
-        <v>48</v>
-      </c>
-      <c r="H2" s="15" t="s">
-        <v>63</v>
-      </c>
-      <c r="I2" s="15" t="s">
-        <v>52</v>
-      </c>
-      <c r="J2" s="12" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>66</v>
-      </c>
-      <c r="B3" t="s">
-        <v>67</v>
-      </c>
-      <c r="C3" t="s">
-        <v>68</v>
-      </c>
-      <c r="D3" s="15" t="s">
-        <v>69</v>
-      </c>
-      <c r="E3" t="s">
-        <v>48</v>
-      </c>
-      <c r="F3" t="s">
-        <v>48</v>
-      </c>
-      <c r="H3" t="s">
-        <v>112</v>
-      </c>
-      <c r="I3" s="15" t="s">
-        <v>70</v>
-      </c>
-      <c r="J3" s="14">
-        <v>43742</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>71</v>
-      </c>
-      <c r="B4" t="s">
-        <v>72</v>
-      </c>
-      <c r="C4" t="s">
-        <v>73</v>
-      </c>
-      <c r="D4" s="15" t="s">
-        <v>62</v>
-      </c>
-      <c r="E4" t="s">
-        <v>48</v>
-      </c>
-      <c r="F4" t="s">
-        <v>94</v>
-      </c>
-      <c r="H4" t="s">
-        <v>51</v>
-      </c>
-      <c r="I4" s="15" t="s">
-        <v>74</v>
-      </c>
-      <c r="J4" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>76</v>
-      </c>
-      <c r="B5" t="s">
-        <v>77</v>
-      </c>
-      <c r="C5" t="s">
-        <v>78</v>
-      </c>
-      <c r="D5" s="15" t="s">
-        <v>62</v>
-      </c>
-      <c r="E5" t="s">
-        <v>48</v>
-      </c>
-      <c r="F5" t="s">
-        <v>94</v>
-      </c>
-      <c r="G5" t="s">
-        <v>72</v>
-      </c>
-      <c r="H5" t="s">
-        <v>92</v>
-      </c>
-      <c r="I5" s="15" t="s">
-        <v>74</v>
-      </c>
-      <c r="J5" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>80</v>
-      </c>
-      <c r="B6" t="s">
-        <v>81</v>
-      </c>
-      <c r="C6" t="s">
-        <v>82</v>
-      </c>
-      <c r="D6" s="15" t="s">
-        <v>62</v>
-      </c>
-      <c r="E6" t="s">
-        <v>48</v>
-      </c>
-      <c r="F6" s="15"/>
-      <c r="I6" s="15" t="s">
-        <v>74</v>
-      </c>
-      <c r="J6" t="s">
-        <v>83</v>
-      </c>
-      <c r="K6" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>87</v>
-      </c>
-      <c r="B7" t="s">
-        <v>84</v>
-      </c>
-      <c r="C7" t="s">
-        <v>85</v>
-      </c>
-      <c r="D7" s="15" t="s">
-        <v>62</v>
-      </c>
-      <c r="E7" t="s">
-        <v>48</v>
-      </c>
-      <c r="F7" s="15"/>
-      <c r="I7" s="15" t="s">
-        <v>64</v>
-      </c>
-      <c r="J7" t="s">
-        <v>86</v>
-      </c>
-      <c r="K7" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>88</v>
-      </c>
-      <c r="B8" t="s">
-        <v>89</v>
-      </c>
-      <c r="C8" t="s">
-        <v>90</v>
-      </c>
-      <c r="D8" s="15" t="s">
-        <v>62</v>
-      </c>
-      <c r="E8" t="s">
-        <v>48</v>
-      </c>
-      <c r="F8" s="15"/>
-      <c r="I8" s="15" t="s">
-        <v>64</v>
-      </c>
-      <c r="J8" t="s">
-        <v>91</v>
-      </c>
-      <c r="K8" t="s">
-        <v>113</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B10"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="21.28515625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="13" t="s">
-        <v>13</v>
-      </c>
-      <c r="B1" s="13" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>71</v>
-      </c>
-      <c r="B2" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>76</v>
-      </c>
-      <c r="B3" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>80</v>
-      </c>
-      <c r="B4" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B5" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B6" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B7" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>88</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
jn: cambio archivo con conflicto
</commit_message>
<xml_diff>
--- a/04_Entregable 2/previo/metadatos y diccionario_AG.xlsx
+++ b/04_Entregable 2/previo/metadatos y diccionario_AG.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Disco_F\!!Personal\Mio\1_WCS 2024\wcs\04_Entregable 2\previo\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MAG\personal\consultorías\wcs\04_Entregable 2\previo\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28770" windowHeight="11385" firstSheet="1" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28770" windowHeight="11385" firstSheet="2" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Metadatos generales" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="119">
   <si>
     <t>Elemento</t>
   </si>
@@ -223,6 +223,9 @@
     <t>Código alfanumérico de entre 14 y 15 caractéres</t>
   </si>
   <si>
+    <t>variable de clasificación</t>
+  </si>
+  <si>
     <t>24281201901783</t>
   </si>
   <si>
@@ -238,6 +241,9 @@
     <t>date</t>
   </si>
   <si>
+    <t>variable temporal</t>
+  </si>
+  <si>
     <t>Provincia</t>
   </si>
   <si>
@@ -247,6 +253,9 @@
     <t>Provincia donde se ingresa el juicio</t>
   </si>
   <si>
+    <t>variable de ubicación</t>
+  </si>
+  <si>
     <t>SANTA ELENA</t>
   </si>
   <si>
@@ -377,18 +386,6 @@
   </si>
   <si>
     <t>TRIBUNAL PENAL</t>
-  </si>
-  <si>
-    <t>Identificación</t>
-  </si>
-  <si>
-    <t>Temporalidad</t>
-  </si>
-  <si>
-    <t>Localización</t>
-  </si>
-  <si>
-    <t>Transacción</t>
   </si>
 </sst>
 </file>
@@ -863,7 +860,7 @@
   <dimension ref="A2:C19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -914,7 +911,7 @@
         <v>30</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="30" x14ac:dyDescent="0.25">
@@ -1086,64 +1083,64 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="B1" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="B2" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="B3" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="B4" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="C4" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="D4" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="E4" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="B5" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="B6" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
       <c r="B7" s="14">
         <v>45535</v>
@@ -1151,7 +1148,7 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
     </row>
   </sheetData>
@@ -1163,8 +1160,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1240,24 +1237,24 @@
         <v>63</v>
       </c>
       <c r="I2" s="15" t="s">
-        <v>116</v>
+        <v>52</v>
       </c>
       <c r="J2" s="12" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B3" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="C3" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="D3" s="15" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="E3" t="s">
         <v>48</v>
@@ -1266,10 +1263,10 @@
         <v>48</v>
       </c>
       <c r="H3" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
       <c r="I3" s="15" t="s">
-        <v>117</v>
+        <v>70</v>
       </c>
       <c r="J3" s="14">
         <v>43742</v>
@@ -1277,13 +1274,13 @@
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="B4" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="C4" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="D4" s="15" t="s">
         <v>62</v>
@@ -1292,27 +1289,27 @@
         <v>48</v>
       </c>
       <c r="F4" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="H4" t="s">
         <v>51</v>
       </c>
       <c r="I4" s="15" t="s">
-        <v>118</v>
+        <v>74</v>
       </c>
       <c r="J4" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="B5" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="C5" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="D5" s="15" t="s">
         <v>62</v>
@@ -1321,30 +1318,30 @@
         <v>48</v>
       </c>
       <c r="F5" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="G5" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="H5" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="I5" s="15" t="s">
-        <v>118</v>
+        <v>74</v>
       </c>
       <c r="J5" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="B6" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="C6" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="D6" s="15" t="s">
         <v>62</v>
@@ -1354,24 +1351,24 @@
       </c>
       <c r="F6" s="15"/>
       <c r="I6" s="15" t="s">
-        <v>6</v>
+        <v>74</v>
       </c>
       <c r="J6" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="K6" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>87</v>
+      </c>
+      <c r="B7" t="s">
         <v>84</v>
       </c>
-      <c r="B7" t="s">
-        <v>81</v>
-      </c>
       <c r="C7" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="D7" s="15" t="s">
         <v>62</v>
@@ -1381,24 +1378,24 @@
       </c>
       <c r="F7" s="15"/>
       <c r="I7" s="15" t="s">
-        <v>119</v>
+        <v>64</v>
       </c>
       <c r="J7" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="K7" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="B8" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="C8" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="D8" s="15" t="s">
         <v>62</v>
@@ -1408,13 +1405,13 @@
       </c>
       <c r="F8" s="15"/>
       <c r="I8" s="15" t="s">
-        <v>6</v>
+        <v>64</v>
       </c>
       <c r="J8" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="K8" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
     </row>
   </sheetData>
@@ -1441,56 +1438,56 @@
         <v>13</v>
       </c>
       <c r="B1" s="13" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="B2" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="B3" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="B4" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
     </row>
   </sheetData>

</xml_diff>